<commit_message>
Added logic of Cache in Designation master
</commit_message>
<xml_diff>
--- a/src/test/TestData/Designation Master.xlsx
+++ b/src/test/TestData/Designation Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.wadhwa\IdeaProjects\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89138C0-1BEC-4C60-891C-6D7389492849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082BEAE-61D9-4F5C-997A-D6C633F5D772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2100,9 +2100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2140,7 +2140,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2246,7 +2246,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2388,7 +2388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2403,7 +2403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G148" sqref="G148"/>
+      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed overlapping issue and reduced skill tagging timimg
</commit_message>
<xml_diff>
--- a/src/test/TestData/Designation Master.xlsx
+++ b/src/test/TestData/Designation Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.wadhwa\IdeaProjects\RMT\src\test\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082BEAE-61D9-4F5C-997A-D6C633F5D772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBB1EB-6314-438B-B1FC-1D541B2B7BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Designation Master" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="659">
   <si>
     <t>DESGN_ID</t>
   </si>
@@ -2010,6 +2010,9 @@
   </si>
   <si>
     <t>//li[text()='Senior Business Analyst']</t>
+  </si>
+  <si>
+    <t>//li[text()='Director, Legal and Risk Management']</t>
   </si>
 </sst>
 </file>
@@ -2396,14 +2399,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,7 +2467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>254</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>489</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -2624,7 +2627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>517</v>
       </c>
@@ -2665,7 +2668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2747,7 +2750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>508</v>
       </c>
@@ -2829,7 +2832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>244</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>412</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>363</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2985,7 +2988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
@@ -3026,7 +3029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>124</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>421</v>
       </c>
@@ -3108,7 +3111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>341</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>115</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>337</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>217</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>396</v>
       </c>
@@ -3305,7 +3308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>388</v>
       </c>
@@ -3342,7 +3345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>399</v>
       </c>
@@ -3379,7 +3382,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>292</v>
       </c>
@@ -3416,7 +3419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>402</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>394</v>
       </c>
@@ -3490,7 +3493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>409</v>
       </c>
@@ -3527,7 +3530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>405</v>
       </c>
@@ -3564,7 +3567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>443</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>502</v>
       </c>
@@ -3683,7 +3686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>153</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>496</v>
       </c>
@@ -3761,7 +3764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>379</v>
       </c>
@@ -3798,7 +3801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>432</v>
       </c>
@@ -3835,7 +3838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>369</v>
       </c>
@@ -3872,7 +3875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>360</v>
       </c>
@@ -3909,7 +3912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>308</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>382</v>
       </c>
@@ -3983,7 +3986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>351</v>
       </c>
@@ -4020,7 +4023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>429</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>299</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>385</v>
       </c>
@@ -4131,7 +4134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>416</v>
       </c>
@@ -4172,7 +4175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>439</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>318</v>
       </c>
@@ -4287,7 +4290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>249</v>
       </c>
@@ -4328,7 +4331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>259</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>193</v>
       </c>
@@ -4410,7 +4413,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>185</v>
       </c>
@@ -4447,7 +4450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>264</v>
       </c>
@@ -4488,7 +4491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>510</v>
       </c>
@@ -4529,7 +4532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>220</v>
       </c>
@@ -4570,7 +4573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>267</v>
       </c>
@@ -4611,7 +4614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>314</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>331</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>334</v>
       </c>
@@ -4710,7 +4713,7 @@
         <v>20</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>520</v>
+        <v>658</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>21</v>
@@ -4722,7 +4725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>285</v>
       </c>
@@ -4763,7 +4766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>290</v>
       </c>
@@ -4804,7 +4807,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>280</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>156</v>
       </c>
@@ -4882,7 +4885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>89</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>180</v>
       </c>
@@ -4960,7 +4963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>159</v>
       </c>
@@ -5227,7 +5230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>426</v>
       </c>
@@ -5264,7 +5267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>471</v>
       </c>
@@ -5338,7 +5341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
@@ -5375,7 +5378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>166</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>169</v>
       </c>
@@ -5449,7 +5452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>224</v>
       </c>
@@ -5490,7 +5493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>69</v>
       </c>
@@ -5531,7 +5534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>213</v>
       </c>
@@ -5572,7 +5575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>142</v>
       </c>
@@ -5613,7 +5616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>56</v>
       </c>
@@ -5654,7 +5657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>127</v>
       </c>
@@ -5695,7 +5698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>129</v>
       </c>
@@ -5736,7 +5739,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>302</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>504</v>
       </c>
@@ -5814,7 +5817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>375</v>
       </c>
@@ -5851,7 +5854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>455</v>
       </c>
@@ -5888,7 +5891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>148</v>
       </c>
@@ -5925,7 +5928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>171</v>
       </c>
@@ -5962,7 +5965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>77</v>
       </c>
@@ -6003,7 +6006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>24</v>
       </c>
@@ -6044,7 +6047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>346</v>
       </c>
@@ -6085,7 +6088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>459</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>435</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>272</v>
       </c>
@@ -6204,7 +6207,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>355</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>234</v>
       </c>
@@ -6286,7 +6289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>447</v>
       </c>
@@ -6323,7 +6326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>451</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>474</v>
       </c>
@@ -6397,7 +6400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>485</v>
       </c>
@@ -6438,7 +6441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>514</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>277</v>
       </c>
@@ -6520,7 +6523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>478</v>
       </c>
@@ -6557,7 +6560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>208</v>
       </c>
@@ -6598,7 +6601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>377</v>
       </c>
@@ -6635,7 +6638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>305</v>
       </c>
@@ -6672,7 +6675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>391</v>
       </c>
@@ -6709,7 +6712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>493</v>
       </c>
@@ -6750,7 +6753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>174</v>
       </c>
@@ -6787,7 +6790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>97</v>
       </c>
@@ -6828,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>134</v>
       </c>
@@ -6869,7 +6872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>100</v>
       </c>
@@ -6910,7 +6913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>239</v>
       </c>
@@ -6951,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>467</v>
       </c>
@@ -6988,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>203</v>
       </c>
@@ -7025,7 +7028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>366</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>45</v>
       </c>
@@ -7103,7 +7106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>181</v>
       </c>
@@ -7144,7 +7147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>131</v>
       </c>
@@ -7185,7 +7188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>53</v>
       </c>
@@ -7226,7 +7229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>463</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>12</v>
       </c>
@@ -7304,7 +7307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>189</v>
       </c>
@@ -7345,7 +7348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>372</v>
       </c>
@@ -7382,7 +7385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>177</v>
       </c>
@@ -7419,7 +7422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>103</v>
       </c>
@@ -7460,7 +7463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>296</v>
       </c>
@@ -7497,7 +7500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>74</v>
       </c>
@@ -7538,7 +7541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>81</v>
       </c>
@@ -7579,7 +7582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>86</v>
       </c>
@@ -7620,7 +7623,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>92</v>
       </c>
@@ -7661,7 +7664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>500</v>
       </c>
@@ -7702,7 +7705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>106</v>
       </c>
@@ -7743,7 +7746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>109</v>
       </c>
@@ -7784,7 +7787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>112</v>
       </c>
@@ -7825,7 +7828,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>311</v>
       </c>
@@ -7862,7 +7865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>32</v>
       </c>
@@ -7904,13 +7907,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:I140" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="GRD00002"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M140">
     <sortCondition ref="C1:C140"/>
   </sortState>

</xml_diff>

<commit_message>
Added Test cases for budget page and reports page + fixed the Null pointer exception handling in DriverManager
</commit_message>
<xml_diff>
--- a/src/test/TestData/Designation Master.xlsx
+++ b/src/test/TestData/Designation Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCAE807-17DC-48F4-B73A-9348AD119EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91D4494-2D7E-42A0-832D-601C2EF106FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Designation Master" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Designation Master'!$J$1:$J$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Designation Master'!$A$1:$M$133</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="619">
   <si>
     <t>DESGN_ID</t>
   </si>
@@ -1079,21 +1079,6 @@
     <t>2021-12-20T17:52:54Z</t>
   </si>
   <si>
-    <t>DG000087</t>
-  </si>
-  <si>
-    <t>P&amp;COO</t>
-  </si>
-  <si>
-    <t>Partner &amp; COO</t>
-  </si>
-  <si>
-    <t>2021-12-06T17:52:54Z</t>
-  </si>
-  <si>
-    <t>06-DEC-21</t>
-  </si>
-  <si>
     <t>DG000091</t>
   </si>
   <si>
@@ -1331,18 +1316,6 @@
     <t>2022-07-26T17:52:54Z</t>
   </si>
   <si>
-    <t>DG000130</t>
-  </si>
-  <si>
-    <t>DRIK</t>
-  </si>
-  <si>
-    <t>Director – IKCC</t>
-  </si>
-  <si>
-    <t>2022-09-15T17:52:54Z</t>
-  </si>
-  <si>
     <t>DG000128</t>
   </si>
   <si>
@@ -1625,9 +1598,6 @@
     <t>(//li[text()='Director FAP'])</t>
   </si>
   <si>
-    <t>(//li[text()='Director – IKCC'])</t>
-  </si>
-  <si>
     <t>(//li[text()='Director Japan Desk'])</t>
   </si>
   <si>
@@ -1805,9 +1775,6 @@
     <t>//li[text()='Partner &amp; CIO']</t>
   </si>
   <si>
-    <t>//li[text()='Partner &amp; COO']</t>
-  </si>
-  <si>
     <t>//li[text()='Partner &amp; Global Delivery Leader']</t>
   </si>
   <si>
@@ -1884,6 +1851,48 @@
   </si>
   <si>
     <t>//li[text()='Client Experience Leader']</t>
+  </si>
+  <si>
+    <t>Associate Consultant</t>
+  </si>
+  <si>
+    <t>//li[text()='Associate Consultant']</t>
+  </si>
+  <si>
+    <t>//li[text()='Chief Operating Officer (designate)']</t>
+  </si>
+  <si>
+    <t>Chief Operating Officer (designate)</t>
+  </si>
+  <si>
+    <t>//li[text()='Director - IKCC']</t>
+  </si>
+  <si>
+    <t>Director - IKCC</t>
+  </si>
+  <si>
+    <t>Partner and National Leader, Financial Services Consulting</t>
+  </si>
+  <si>
+    <t>//li[text()='Partner and National Leader, Financial Services Consulting']</t>
+  </si>
+  <si>
+    <t>Chief Information Officer</t>
+  </si>
+  <si>
+    <t>Partner, COO</t>
+  </si>
+  <si>
+    <t>Partner,CPCO</t>
+  </si>
+  <si>
+    <t>//li[text()='Chief Information Officer']</t>
+  </si>
+  <si>
+    <t>//li[text()='Partner, COO']</t>
+  </si>
+  <si>
+    <t>//li[text()='Partner,CPCO']</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +1916,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1920,8 +1929,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1944,11 +1959,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1956,6 +1997,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2284,11 +2338,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J114" sqref="J114"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2337,7 +2391,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
@@ -2378,7 +2432,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>21</v>
@@ -2392,19 +2446,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -2415,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>21</v>
@@ -2456,7 +2510,7 @@
         <v>44</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>21</v>
@@ -2497,7 +2551,7 @@
         <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>21</v>
@@ -2538,7 +2592,7 @@
         <v>44</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>21</v>
@@ -2579,7 +2633,7 @@
         <v>31</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>21</v>
@@ -2620,7 +2674,7 @@
         <v>27</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
@@ -2634,19 +2688,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
@@ -2657,7 +2711,7 @@
         <v>27</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>21</v>
@@ -2671,13 +2725,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -2694,7 +2748,7 @@
         <v>48</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>21</v>
@@ -2735,7 +2789,7 @@
         <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>21</v>
@@ -2776,7 +2830,7 @@
         <v>38</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>21</v>
@@ -2817,7 +2871,7 @@
         <v>38</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>21</v>
@@ -2831,34 +2885,34 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>21</v>
@@ -2899,7 +2953,7 @@
         <v>27</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>21</v>
@@ -2940,7 +2994,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>21</v>
@@ -2977,7 +3031,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>21</v>
@@ -3018,7 +3072,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>21</v>
@@ -3032,13 +3086,13 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -3055,7 +3109,7 @@
         <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>21</v>
@@ -3069,13 +3123,13 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -3092,7 +3146,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>21</v>
@@ -3106,13 +3160,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -3129,7 +3183,7 @@
         <v>27</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>21</v>
@@ -3166,7 +3220,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>21</v>
@@ -3180,13 +3234,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -3203,7 +3257,7 @@
         <v>27</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>21</v>
@@ -3217,13 +3271,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>285</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -3240,7 +3294,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>21</v>
@@ -3254,19 +3308,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -3277,7 +3331,7 @@
         <v>31</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>21</v>
@@ -3291,19 +3345,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -3314,7 +3368,7 @@
         <v>38</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>21</v>
@@ -3328,19 +3382,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -3351,7 +3405,7 @@
         <v>27</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>21</v>
@@ -3392,7 +3446,7 @@
         <v>52</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>21</v>
@@ -3429,7 +3483,7 @@
         <v>44</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>21</v>
@@ -3443,13 +3497,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -3466,7 +3520,7 @@
         <v>38</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>21</v>
@@ -3480,13 +3534,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -3503,7 +3557,7 @@
         <v>52</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>21</v>
@@ -3517,13 +3571,13 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -3540,7 +3594,7 @@
         <v>38</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>21</v>
@@ -3554,13 +3608,13 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -3577,7 +3631,7 @@
         <v>48</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>21</v>
@@ -3614,7 +3668,7 @@
         <v>31</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>21</v>
@@ -3628,13 +3682,13 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>17</v>
@@ -3651,7 +3705,7 @@
         <v>31</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>21</v>
@@ -3688,7 +3742,7 @@
         <v>38</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>21</v>
@@ -3702,13 +3756,13 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
@@ -3725,7 +3779,7 @@
         <v>52</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>21</v>
@@ -3762,7 +3816,7 @@
         <v>52</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>21</v>
@@ -3776,13 +3830,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>17</v>
@@ -3799,7 +3853,7 @@
         <v>31</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>21</v>
@@ -3813,34 +3867,34 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>21</v>
@@ -3881,7 +3935,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>21</v>
@@ -3895,19 +3949,19 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>431</v>
+        <v>310</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>432</v>
+        <v>311</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>433</v>
+        <v>312</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>434</v>
+        <v>309</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
@@ -3918,7 +3972,7 @@
         <v>20</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>21</v>
@@ -3932,30 +3986,34 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>310</v>
+        <v>241</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>312</v>
+        <v>243</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G43" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H43" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="I43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>21</v>
@@ -3969,13 +4027,13 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>17</v>
@@ -3987,16 +4045,16 @@
         <v>17</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>21</v>
@@ -4010,34 +4068,34 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>251</v>
+        <v>185</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>252</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>253</v>
+        <v>186</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>255</v>
+        <v>189</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>21</v>
@@ -4051,34 +4109,30 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H46" s="1"/>
       <c r="I46" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>21</v>
@@ -4092,30 +4146,34 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>177</v>
+        <v>256</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>178</v>
+        <v>257</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>179</v>
+        <v>258</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H47" s="1"/>
+        <v>254</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="I47" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>21</v>
@@ -4129,13 +4187,13 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>256</v>
+        <v>212</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>257</v>
+        <v>131</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>17</v>
@@ -4147,16 +4205,16 @@
         <v>17</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>21</v>
@@ -4170,13 +4228,13 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>131</v>
+        <v>260</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>17</v>
@@ -4188,16 +4246,16 @@
         <v>17</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>21</v>
@@ -4211,34 +4269,30 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>259</v>
+        <v>306</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>260</v>
+        <v>307</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>261</v>
+        <v>308</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>263</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>21</v>
@@ -4252,19 +4306,19 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -4275,7 +4329,7 @@
         <v>20</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>21</v>
@@ -4289,13 +4343,13 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>17</v>
@@ -4312,7 +4366,7 @@
         <v>20</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>536</v>
+        <v>598</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>21</v>
@@ -4326,30 +4380,34 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>327</v>
+        <v>278</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F53" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G53" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H53" s="1"/>
+        <v>280</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="I53" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>609</v>
+        <v>518</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>21</v>
@@ -4363,13 +4421,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>17</v>
@@ -4390,7 +4448,7 @@
         <v>20</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>527</v>
+        <v>547</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>21</v>
@@ -4404,13 +4462,13 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>17</v>
@@ -4422,16 +4480,16 @@
         <v>17</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>21</v>
@@ -4445,34 +4503,30 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>272</v>
+        <v>149</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>273</v>
+        <v>150</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>274</v>
+        <v>151</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>276</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>21</v>
@@ -4486,30 +4540,34 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F57" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G57" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H57" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I57" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>21</v>
@@ -4523,34 +4581,34 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>21</v>
@@ -4564,34 +4622,30 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>155</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>21</v>
@@ -4605,30 +4659,34 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>224</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G60" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H60" s="1"/>
+        <v>224</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="I60" s="1" t="s">
         <v>194</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>21</v>
@@ -4642,34 +4700,30 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>222</v>
+        <v>314</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>223</v>
+        <v>315</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>225</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
         <v>194</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>21</v>
@@ -4683,13 +4737,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>17</v>
@@ -4706,7 +4760,7 @@
         <v>194</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>21</v>
@@ -4720,13 +4774,13 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>17</v>
@@ -4743,7 +4797,7 @@
         <v>194</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>21</v>
@@ -4757,19 +4811,19 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>317</v>
+        <v>413</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>318</v>
+        <v>414</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>319</v>
+        <v>415</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
@@ -4777,10 +4831,10 @@
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
-        <v>194</v>
+        <v>52</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>21</v>
@@ -4794,19 +4848,19 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>418</v>
+        <v>454</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>419</v>
+        <v>455</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>420</v>
+        <v>456</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>287</v>
+        <v>453</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
@@ -4814,10 +4868,10 @@
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>21</v>
@@ -4831,19 +4885,19 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>464</v>
+        <v>420</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -4851,10 +4905,10 @@
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
-        <v>27</v>
+        <v>194</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>21</v>
@@ -4868,19 +4922,19 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>474</v>
+        <v>156</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>425</v>
+        <v>157</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>475</v>
+        <v>158</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>476</v>
+        <v>144</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -4888,10 +4942,10 @@
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
-        <v>194</v>
+        <v>44</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>21</v>
@@ -4905,13 +4959,13 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>17</v>
@@ -4925,10 +4979,10 @@
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>21</v>
@@ -4942,13 +4996,13 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>17</v>
@@ -4962,10 +5016,10 @@
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>21</v>
@@ -4979,30 +5033,34 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>162</v>
+        <v>216</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F70" s="1"/>
+        <v>219</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G70" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H70" s="1"/>
+        <v>219</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="I70" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>21</v>
@@ -5016,34 +5074,34 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>216</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>217</v>
+        <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>218</v>
+        <v>71</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>219</v>
+        <v>16</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>219</v>
+        <v>72</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>220</v>
+        <v>73</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>21</v>
@@ -5057,34 +5115,34 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>70</v>
+        <v>206</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>71</v>
+        <v>206</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>21</v>
@@ -5098,34 +5156,34 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>206</v>
+        <v>137</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>21</v>
@@ -5139,34 +5197,34 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>21</v>
@@ -5180,34 +5238,30 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>56</v>
+        <v>294</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>57</v>
+        <v>295</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>58</v>
+        <v>296</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H75" s="1"/>
       <c r="I75" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>21</v>
@@ -5221,13 +5275,13 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>294</v>
+        <v>362</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>296</v>
+        <v>363</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>17</v>
@@ -5244,7 +5298,7 @@
         <v>38</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>21</v>
@@ -5258,19 +5312,19 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>367</v>
+        <v>438</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>295</v>
+        <v>439</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>368</v>
+        <v>440</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>287</v>
+        <v>441</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -5278,10 +5332,10 @@
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>21</v>
@@ -5295,19 +5349,19 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>447</v>
+        <v>141</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>448</v>
+        <v>142</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>449</v>
+        <v>143</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>450</v>
+        <v>144</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -5315,10 +5369,10 @@
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>21</v>
@@ -5332,13 +5386,13 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>17</v>
@@ -5355,7 +5409,7 @@
         <v>44</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>21</v>
@@ -5369,30 +5423,34 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F80" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G80" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H80" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I80" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>21</v>
@@ -5406,19 +5464,19 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>17</v>
@@ -5430,10 +5488,10 @@
         <v>19</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>21</v>
@@ -5447,34 +5505,34 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>24</v>
+        <v>338</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>25</v>
+        <v>339</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>26</v>
+        <v>340</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>16</v>
+        <v>341</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>18</v>
+        <v>341</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>19</v>
+        <v>342</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>21</v>
@@ -5488,34 +5546,34 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>338</v>
+        <v>442</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>339</v>
+        <v>443</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>340</v>
+        <v>444</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>341</v>
+        <v>445</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>341</v>
+        <v>18</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>342</v>
+        <v>19</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>21</v>
@@ -5529,34 +5587,30 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>451</v>
+        <v>422</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>452</v>
+        <v>423</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>453</v>
+        <v>424</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H84" s="1"/>
       <c r="I84" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>21</v>
@@ -5570,30 +5624,34 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>427</v>
+        <v>264</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>428</v>
+        <v>265</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>429</v>
+        <v>266</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G85" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H85" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="I85" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>21</v>
@@ -5607,34 +5665,34 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>21</v>
@@ -5648,34 +5706,30 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>347</v>
+        <v>430</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>348</v>
+        <v>431</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>349</v>
+        <v>432</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>351</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H87" s="1"/>
       <c r="I87" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>21</v>
@@ -5689,34 +5743,30 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>226</v>
+        <v>434</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>227</v>
+        <v>435</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>228</v>
+        <v>436</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>230</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H88" s="1"/>
       <c r="I88" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>21</v>
@@ -5730,19 +5780,19 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
@@ -5753,7 +5803,7 @@
         <v>27</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>21</v>
@@ -5767,30 +5817,34 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>443</v>
+        <v>468</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>444</v>
+        <v>339</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>445</v>
+        <v>469</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="F90" s="1"/>
+        <v>470</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G90" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H90" s="1"/>
+        <v>470</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="I90" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>21</v>
@@ -5804,30 +5858,34 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>466</v>
+        <v>269</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>467</v>
+        <v>270</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>468</v>
+        <v>271</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F91" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G91" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H91" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="I91" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>21</v>
@@ -5841,34 +5899,30 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>339</v>
+        <v>462</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>480</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H92" s="1"/>
       <c r="I92" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>21</v>
@@ -5882,34 +5936,34 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>269</v>
+        <v>200</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>267</v>
+        <v>18</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>21</v>
@@ -5923,19 +5977,19 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>470</v>
+        <v>364</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>471</v>
+        <v>295</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>472</v>
+        <v>365</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>473</v>
+        <v>287</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
@@ -5946,7 +6000,7 @@
         <v>38</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>21</v>
@@ -5960,34 +6014,30 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>200</v>
+        <v>297</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>201</v>
+        <v>298</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>202</v>
+        <v>299</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>204</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H95" s="1"/>
       <c r="I95" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>21</v>
@@ -6001,13 +6051,13 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>295</v>
+        <v>379</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>17</v>
@@ -6021,10 +6071,10 @@
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>21</v>
@@ -6038,19 +6088,19 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>297</v>
+        <v>167</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>298</v>
+        <v>168</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>299</v>
+        <v>169</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>287</v>
+        <v>144</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
@@ -6058,10 +6108,10 @@
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>21</v>
@@ -6075,30 +6125,34 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>383</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>384</v>
+        <v>98</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>385</v>
+        <v>99</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F98" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G98" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H98" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I98" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>21</v>
@@ -6112,30 +6166,34 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G99" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H99" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="I99" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="K99" s="1" t="s">
         <v>21</v>
@@ -6149,13 +6207,13 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>17</v>
@@ -6167,16 +6225,16 @@
         <v>17</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>21</v>
@@ -6190,13 +6248,13 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>127</v>
+        <v>231</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>128</v>
+        <v>232</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>17</v>
@@ -6208,16 +6266,16 @@
         <v>17</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>72</v>
+        <v>234</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>73</v>
+        <v>235</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>21</v>
@@ -6231,34 +6289,30 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>100</v>
+        <v>450</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>101</v>
+        <v>451</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>102</v>
+        <v>452</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>453</v>
+      </c>
+      <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H102" s="1"/>
       <c r="I102" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>21</v>
@@ -6272,34 +6326,30 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>235</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H103" s="1"/>
       <c r="I103" s="1" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>21</v>
@@ -6313,19 +6363,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>459</v>
+        <v>353</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>460</v>
+        <v>354</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>461</v>
+        <v>355</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>462</v>
+        <v>287</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
@@ -6333,10 +6383,10 @@
       </c>
       <c r="H104" s="1"/>
       <c r="I104" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>21</v>
@@ -6350,30 +6400,34 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>195</v>
+        <v>45</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>197</v>
+        <v>47</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F105" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G105" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H105" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I105" s="1" t="s">
-        <v>199</v>
+        <v>48</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>607</v>
+        <v>546</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>21</v>
@@ -6387,30 +6441,34 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>358</v>
+        <v>173</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>359</v>
+        <v>174</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>360</v>
+        <v>175</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>176</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G106" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H106" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I106" s="1" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>608</v>
+        <v>545</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>21</v>
@@ -6424,19 +6482,19 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>17</v>
@@ -6448,10 +6506,10 @@
         <v>19</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>556</v>
+        <v>544</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>21</v>
@@ -6465,19 +6523,19 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>174</v>
+        <v>54</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>175</v>
+        <v>55</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>176</v>
+        <v>16</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>17</v>
@@ -6489,10 +6547,10 @@
         <v>19</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>21</v>
@@ -6506,34 +6564,30 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>124</v>
+        <v>446</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>125</v>
+        <v>447</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>126</v>
+        <v>448</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H109" s="1"/>
       <c r="I109" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>21</v>
@@ -6547,13 +6601,13 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>15</v>
@@ -6571,10 +6625,10 @@
         <v>19</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>21</v>
@@ -6588,30 +6642,34 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>455</v>
+        <v>181</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>456</v>
+        <v>182</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>457</v>
+        <v>183</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="F111" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G111" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H111" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I111" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>21</v>
@@ -6625,34 +6683,30 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>12</v>
+        <v>359</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>13</v>
+        <v>360</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>14</v>
+        <v>361</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="F112" s="1"/>
       <c r="G112" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H112" s="1"/>
       <c r="I112" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>21</v>
@@ -6666,34 +6720,30 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F113" s="1"/>
       <c r="G113" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H113" s="1"/>
       <c r="I113" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>21</v>
@@ -6707,30 +6757,34 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>364</v>
+        <v>103</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>365</v>
+        <v>104</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>366</v>
+        <v>105</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F114" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G114" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H114" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I114" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>21</v>
@@ -6744,19 +6798,19 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>170</v>
+        <v>288</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>172</v>
+        <v>290</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>144</v>
+        <v>287</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1" t="s">
@@ -6764,10 +6818,10 @@
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>21</v>
@@ -6781,34 +6835,34 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="K116" s="1" t="s">
         <v>21</v>
@@ -6822,30 +6876,34 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>288</v>
+        <v>81</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>289</v>
+        <v>82</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>290</v>
+        <v>83</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F117" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G117" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H117" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="I117" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>21</v>
@@ -6859,19 +6917,19 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>17</v>
@@ -6886,7 +6944,7 @@
         <v>44</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>21</v>
@@ -6900,16 +6958,16 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>85</v>
@@ -6918,16 +6976,16 @@
         <v>17</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>21</v>
@@ -6941,34 +6999,34 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="K120" s="1" t="s">
         <v>21</v>
@@ -6982,34 +7040,34 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>542</v>
+        <v>530</v>
       </c>
       <c r="K121" s="1" t="s">
         <v>21</v>
@@ -7023,13 +7081,13 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>17</v>
@@ -7050,7 +7108,7 @@
         <v>44</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="K122" s="1" t="s">
         <v>21</v>
@@ -7064,34 +7122,30 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>109</v>
+        <v>303</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>110</v>
+        <v>304</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>111</v>
+        <v>305</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="F123" s="1"/>
       <c r="G123" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H123" s="1"/>
       <c r="I123" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="K123" s="1" t="s">
         <v>21</v>
@@ -7105,19 +7159,19 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>17</v>
@@ -7129,10 +7183,10 @@
         <v>19</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>21</v>
@@ -7146,30 +7200,34 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>303</v>
+        <v>32</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>304</v>
+        <v>600</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>305</v>
+        <v>601</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F125" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G125" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H125" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I125" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>538</v>
+        <v>599</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>21</v>
@@ -7186,10 +7244,10 @@
         <v>32</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>33</v>
+        <v>600</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>34</v>
+        <v>603</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>15</v>
@@ -7210,7 +7268,7 @@
         <v>31</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>537</v>
+        <v>604</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>21</v>
@@ -7227,10 +7285,10 @@
         <v>32</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>15</v>
@@ -7248,10 +7306,10 @@
         <v>19</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J127" s="1" t="s">
-        <v>610</v>
+        <v>52</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>606</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>21</v>
@@ -7268,10 +7326,10 @@
         <v>32</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>15</v>
@@ -7291,23 +7349,228 @@
       <c r="I128" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J128" s="1" t="s">
+      <c r="J128" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H130" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="K130" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L130" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M130" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A132" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L132" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="K128" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L128" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M128" s="1" t="s">
+      <c r="D133" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M133" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="J1:J128" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M126">
-    <sortCondition ref="C1:C126"/>
+  <autoFilter ref="A1:M133" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M124">
+    <sortCondition ref="C1:C124"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>